<commit_message>
Update xlsx & Fix a bug
</commit_message>
<xml_diff>
--- a/fortune_city.xlsx
+++ b/fortune_city.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linyuxiang/Desktop/code/fortune_city/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8371BA31-E253-F442-9D68-0046382405CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18070C84-15F7-A449-8E02-DE063305C903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28260" windowHeight="16000" activeTab="1" xr2:uid="{69F0C2EB-5539-304A-915E-BB8FA7D0757C}"/>
   </bookViews>
@@ -779,7 +779,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>